<commit_message>
Readme & misc updates
</commit_message>
<xml_diff>
--- a/$BOWL.xlsx
+++ b/$BOWL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2EF68D-055E-4AA9-9E49-DD1F5C99A74F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB3FF4E-1EE4-45FB-9DF8-4E5FE2DCDE15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F8D34B35-9CB9-43D1-AD57-473E4BE04DBD}"/>
   </bookViews>
@@ -387,8 +387,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
-    <numFmt numFmtId="173" formatCode="0.0\x"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -582,38 +582,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -634,8 +613,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -644,12 +623,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -665,28 +638,56 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1126,7 +1127,7 @@
   <dimension ref="A2:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+      <selection activeCell="K21" sqref="K21:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1145,416 +1146,422 @@
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="G5" s="3" t="s">
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="G5" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="5"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="45"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>16.05</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19"/>
+      <c r="D6" s="16"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="18">
         <v>165.83689699999999</v>
       </c>
-      <c r="D7" s="23" t="str">
+      <c r="D7" s="16" t="str">
         <f>$C$30</f>
         <v>Q223</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="19"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="18">
         <f>C6*C7</f>
         <v>2661.6821968499999</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
+      <c r="D8" s="16"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="18">
         <f>'Financial Models'!L74</f>
         <v>91.570999999999998</v>
       </c>
-      <c r="D9" s="23" t="str">
+      <c r="D9" s="16" t="str">
         <f t="shared" ref="D9:D11" si="0">$C$30</f>
         <v>Q223</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="18">
         <f>'Financial Models'!L75</f>
         <v>882.67700000000002</v>
       </c>
-      <c r="D10" s="23" t="str">
+      <c r="D10" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Q223</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="19"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="18">
         <f>C9-C10</f>
         <v>-791.10599999999999</v>
       </c>
-      <c r="D11" s="23" t="str">
+      <c r="D11" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Q223</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="19">
         <f>C8-C11</f>
         <v>3452.7881968499996</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="19"/>
+      <c r="D12" s="17"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="19"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="19"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="12"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="19"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="19"/>
+      <c r="D16" s="40"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="12"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="19"/>
+      <c r="D17" s="40"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="12"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="19"/>
+      <c r="D18" s="40"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="19"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="12"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="19"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="12"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G21" s="17"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="19"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="12"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="22"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="15"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="39">
         <v>1997</v>
       </c>
-      <c r="D24" s="11"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="39">
         <v>2021</v>
       </c>
-      <c r="D25" s="11"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B26" s="15"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="39">
         <f>'Financial Models'!L36</f>
         <v>327</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="15"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="49">
+      <c r="D30" s="38">
         <v>44958</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="31"/>
+      <c r="D31" s="47"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="45"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="48">
         <f>C6/'Financial Models'!L72</f>
         <v>16.995954373839119</v>
       </c>
-      <c r="D35" s="44"/>
+      <c r="D35" s="49"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="40"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="11"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="40"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="40"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="14"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
@@ -1571,12 +1578,6 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{21B9D159-E60F-4CDF-8511-BDBA3019D342}"/>
@@ -1592,10 +1593,10 @@
   <dimension ref="B1:AC86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J46" sqref="J46"/>
+      <selection pane="bottomRight" activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1605,242 +1606,278 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="29" t="s">
+    <row r="1" spans="2:29" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="Q1" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="R1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="29" t="s">
+      <c r="S1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="T1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="29" t="s">
+      <c r="U1" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="V1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="29" t="s">
+      <c r="W1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="X1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" s="29" t="s">
+      <c r="Y1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="29" t="s">
+      <c r="Z1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AA1" s="29" t="s">
+      <c r="AA1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="29" t="s">
+      <c r="AB1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AC1" s="29" t="s">
+      <c r="AC1" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="2:29" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="33"/>
-      <c r="H2" s="35">
+    <row r="2" spans="2:29" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="24"/>
+      <c r="G2" s="26">
+        <v>44465</v>
+      </c>
+      <c r="H2" s="26">
         <v>44556</v>
       </c>
-      <c r="J2" s="35">
+      <c r="J2" s="26">
         <v>44745</v>
       </c>
-      <c r="L2" s="35">
+      <c r="K2" s="26">
+        <v>44836</v>
+      </c>
+      <c r="L2" s="26">
         <v>44927</v>
       </c>
     </row>
-    <row r="3" spans="2:29" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="33"/>
-      <c r="L3" s="48">
+    <row r="3" spans="2:29" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="24"/>
+      <c r="L3" s="37">
         <v>44958</v>
       </c>
     </row>
-    <row r="4" spans="2:29" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="45" t="s">
+    <row r="4" spans="2:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="H4" s="47">
+      <c r="G4" s="36">
+        <v>92.61</v>
+      </c>
+      <c r="H4" s="36">
         <v>103.532</v>
       </c>
-      <c r="L4" s="47">
+      <c r="K4" s="36">
+        <v>115.327</v>
+      </c>
+      <c r="L4" s="36">
         <v>131.42599999999999</v>
       </c>
     </row>
-    <row r="5" spans="2:29" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="45" t="s">
+    <row r="5" spans="2:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="H5" s="47">
+      <c r="G5" s="36">
+        <v>60.244999999999997</v>
+      </c>
+      <c r="H5" s="36">
         <v>72.774000000000001</v>
       </c>
-      <c r="L5" s="47">
+      <c r="K5" s="36">
+        <v>79.022999999999996</v>
+      </c>
+      <c r="L5" s="36">
         <v>100.657</v>
       </c>
     </row>
-    <row r="6" spans="2:29" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="45" t="s">
+    <row r="6" spans="2:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="H6" s="47">
+      <c r="G6" s="36">
+        <v>23.710999999999999</v>
+      </c>
+      <c r="H6" s="36">
         <v>26.474</v>
       </c>
-      <c r="L6" s="47">
+      <c r="K6" s="36">
+        <v>30.809000000000001</v>
+      </c>
+      <c r="L6" s="36">
         <v>36.747999999999998</v>
       </c>
     </row>
-    <row r="7" spans="2:29" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="45" t="s">
+    <row r="7" spans="2:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="H7" s="47">
+      <c r="G7" s="36">
+        <v>4.4119999999999999</v>
+      </c>
+      <c r="H7" s="36">
         <v>2.41</v>
       </c>
-      <c r="L7" s="47">
+      <c r="K7" s="36">
+        <v>5.101</v>
+      </c>
+      <c r="L7" s="36">
         <v>4.5540000000000003</v>
       </c>
     </row>
-    <row r="8" spans="2:29" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="38" t="s">
+    <row r="8" spans="2:29" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="29">
         <f t="shared" ref="C8:K8" si="0">SUM(C4:C7)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="38">
+        <v>180.97799999999998</v>
+      </c>
+      <c r="H8" s="29">
         <f t="shared" si="0"/>
         <v>205.18999999999997</v>
       </c>
-      <c r="I8" s="38">
+      <c r="I8" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="38">
+      <c r="J8" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K8" s="38">
+      <c r="K8" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="38">
+        <v>230.26</v>
+      </c>
+      <c r="L8" s="29">
         <f>SUM(L4:L7)</f>
         <v>273.38499999999993</v>
       </c>
     </row>
-    <row r="9" spans="2:29" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="39" t="s">
+    <row r="9" spans="2:29" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="39">
+      <c r="G9" s="30">
+        <v>126.86799999999999</v>
+      </c>
+      <c r="H9" s="30">
         <v>141.38300000000001</v>
       </c>
-      <c r="L9" s="39">
+      <c r="K9" s="30">
+        <v>165.202</v>
+      </c>
+      <c r="L9" s="30">
         <v>179.70599999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:29" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="38" t="s">
+    <row r="10" spans="2:29" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="29">
         <f t="shared" ref="C10:K10" si="1">C8-C9</f>
         <v>0</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="38">
+        <v>54.109999999999985</v>
+      </c>
+      <c r="H10" s="29">
         <f t="shared" si="1"/>
         <v>63.80699999999996</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10" s="29">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="38">
+        <v>65.057999999999993</v>
+      </c>
+      <c r="L10" s="29">
         <f>L8-L9</f>
         <v>93.678999999999945</v>
       </c>
@@ -1849,10 +1886,16 @@
       <c r="B11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="39">
+      <c r="G11" s="30">
+        <v>21.414999999999999</v>
+      </c>
+      <c r="H11" s="30">
         <v>93.283000000000001</v>
       </c>
-      <c r="L11" s="39">
+      <c r="K11" s="30">
+        <v>32.494</v>
+      </c>
+      <c r="L11" s="30">
         <v>34.451999999999998</v>
       </c>
     </row>
@@ -1860,10 +1903,16 @@
       <c r="B12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="39">
-        <v>0</v>
-      </c>
-      <c r="L12" s="39">
+      <c r="G12" s="30">
+        <v>0</v>
+      </c>
+      <c r="H12" s="30">
+        <v>0</v>
+      </c>
+      <c r="K12" s="30">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="L12" s="30">
         <v>0</v>
       </c>
     </row>
@@ -1871,10 +1920,16 @@
       <c r="B13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="39">
+      <c r="G13" s="30">
+        <v>-0.03</v>
+      </c>
+      <c r="H13" s="30">
         <v>-0.124</v>
       </c>
-      <c r="L13" s="39">
+      <c r="K13" s="30">
+        <v>-0.155</v>
+      </c>
+      <c r="L13" s="30">
         <v>-1.823</v>
       </c>
     </row>
@@ -1882,10 +1937,16 @@
       <c r="B14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="39">
+      <c r="G14" s="30">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="H14" s="30">
         <v>3.3319999999999999</v>
       </c>
-      <c r="L14" s="39">
+      <c r="K14" s="30">
+        <v>1.3620000000000001</v>
+      </c>
+      <c r="L14" s="30">
         <v>0.61399999999999999</v>
       </c>
     </row>
@@ -1893,43 +1954,43 @@
       <c r="B15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="29">
         <f t="shared" ref="C15:K15" si="2">C10-SUM(C11:C14)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="29">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="38">
+        <v>32.24799999999999</v>
+      </c>
+      <c r="H15" s="29">
         <f t="shared" si="2"/>
         <v>-32.68400000000004</v>
       </c>
-      <c r="I15" s="38">
+      <c r="I15" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J15" s="38">
+      <c r="J15" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K15" s="38">
+      <c r="K15" s="29">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="38">
+        <v>31.272999999999989</v>
+      </c>
+      <c r="L15" s="29">
         <f>L10-SUM(L11:L14)</f>
         <v>60.43599999999995</v>
       </c>
@@ -1938,10 +1999,16 @@
       <c r="B16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H16" s="39">
+      <c r="G16" s="30">
+        <v>22.928000000000001</v>
+      </c>
+      <c r="H16" s="30">
         <v>23.88</v>
       </c>
-      <c r="L16" s="39">
+      <c r="K16" s="30">
+        <v>23.57</v>
+      </c>
+      <c r="L16" s="30">
         <v>27.379000000000001</v>
       </c>
     </row>
@@ -1949,10 +2016,16 @@
       <c r="B17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="39">
+      <c r="G17" s="30">
+        <v>0</v>
+      </c>
+      <c r="H17" s="30">
         <v>-22.542000000000002</v>
       </c>
-      <c r="L17" s="39">
+      <c r="K17" s="30">
+        <v>40.76</v>
+      </c>
+      <c r="L17" s="30">
         <v>30.776</v>
       </c>
     </row>
@@ -1960,10 +2033,16 @@
       <c r="B18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="39">
+      <c r="G18" s="30">
+        <v>0</v>
+      </c>
+      <c r="H18" s="30">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L18" s="39">
+      <c r="K18" s="30">
+        <v>0</v>
+      </c>
+      <c r="L18" s="30">
         <v>0</v>
       </c>
     </row>
@@ -1971,10 +2050,16 @@
       <c r="B19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H19" s="39">
-        <v>0</v>
-      </c>
-      <c r="L19" s="39">
+      <c r="G19" s="30">
+        <v>0</v>
+      </c>
+      <c r="H19" s="30">
+        <v>0</v>
+      </c>
+      <c r="K19" s="30">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L19" s="30">
         <v>-0.67800000000000005</v>
       </c>
     </row>
@@ -1982,11 +2067,19 @@
       <c r="B20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="39">
+      <c r="G20" s="30">
+        <f>SUM(G16:G19)</f>
+        <v>22.928000000000001</v>
+      </c>
+      <c r="H20" s="30">
         <f>SUM(H16:H19)</f>
         <v>1.4079999999999975</v>
       </c>
-      <c r="L20" s="39">
+      <c r="K20" s="30">
+        <f>SUM(K16:K19)</f>
+        <v>64.378</v>
+      </c>
+      <c r="L20" s="30">
         <f>SUM(L16:L19)</f>
         <v>57.477000000000004</v>
       </c>
@@ -1995,43 +2088,43 @@
       <c r="B21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="30">
         <f t="shared" ref="C21:K21" si="3">C15-C20</f>
         <v>0</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E21" s="39">
+      <c r="E21" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="39">
+        <v>9.3199999999999896</v>
+      </c>
+      <c r="H21" s="30">
         <f t="shared" si="3"/>
         <v>-34.092000000000034</v>
       </c>
-      <c r="I21" s="39">
+      <c r="I21" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J21" s="39">
+      <c r="J21" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K21" s="39">
+      <c r="K21" s="30">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="39">
+        <v>-33.105000000000011</v>
+      </c>
+      <c r="L21" s="30">
         <f>L15-L20</f>
         <v>2.9589999999999463</v>
       </c>
@@ -2040,10 +2133,16 @@
       <c r="B22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H22" s="39">
+      <c r="G22" s="30">
+        <v>-6.2439999999999998</v>
+      </c>
+      <c r="H22" s="30">
         <v>0.36199999999999999</v>
       </c>
-      <c r="L22" s="39">
+      <c r="K22" s="30">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="L22" s="30">
         <v>1.524</v>
       </c>
     </row>
@@ -2051,68 +2150,82 @@
       <c r="B23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="29">
         <f t="shared" ref="C23:K23" si="4">C21-C22</f>
         <v>0</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="38">
+        <v>15.563999999999989</v>
+      </c>
+      <c r="H23" s="29">
         <f t="shared" si="4"/>
         <v>-34.454000000000036</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J23" s="38">
+      <c r="J23" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K23" s="38">
+      <c r="K23" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="38">
+        <v>-33.534000000000013</v>
+      </c>
+      <c r="L23" s="29">
         <f>L21-L22</f>
         <v>1.4349999999999463</v>
       </c>
     </row>
-    <row r="24" spans="2:12" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="42" t="s">
+    <row r="24" spans="2:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="H24" s="42">
+      <c r="G24" s="33">
+        <f>G23/G25</f>
+        <v>0.10598690643587028</v>
+      </c>
+      <c r="H24" s="33">
         <f>H23/H25</f>
         <v>-0.23161588725529672</v>
       </c>
-      <c r="L24" s="42">
+      <c r="K24" s="33">
+        <f>K23/K25</f>
+        <v>-0.20591374525338091</v>
+      </c>
+      <c r="L24" s="33">
         <f>L23/L25</f>
         <v>8.8319569523398513E-3</v>
       </c>
     </row>
-    <row r="25" spans="2:12" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="39" t="s">
+    <row r="25" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="39">
+      <c r="G25" s="30">
+        <v>146.84832800000001</v>
+      </c>
+      <c r="H25" s="30">
         <v>148.754908</v>
       </c>
-      <c r="L25" s="39">
+      <c r="K25" s="30">
+        <v>162.85459700000001</v>
+      </c>
+      <c r="L25" s="30">
         <v>162.47814700000001</v>
       </c>
     </row>
@@ -2120,7 +2233,11 @@
       <c r="B27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="L27" s="40">
+      <c r="K27" s="31">
+        <f>K10/G10-1</f>
+        <v>0.20232858990944402</v>
+      </c>
+      <c r="L27" s="31">
         <f>L10/H10-1</f>
         <v>0.46816180042942013</v>
       </c>
@@ -2129,63 +2246,101 @@
       <c r="B28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H28" s="41"/>
-      <c r="L28" s="41"/>
-    </row>
-    <row r="30" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="41" t="s">
+      <c r="H28" s="32">
+        <f>H8/G8-1</f>
+        <v>0.13378421686613828</v>
+      </c>
+      <c r="L28" s="32">
+        <f>L8/K8-1</f>
+        <v>0.1872882828107354</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="H30" s="41">
+      <c r="G30" s="32">
+        <f t="shared" ref="G30:H30" si="5">G10/G8</f>
+        <v>0.29898661715788655</v>
+      </c>
+      <c r="H30" s="32">
         <f>H10/H8</f>
         <v>0.31096544665919379</v>
       </c>
-      <c r="L30" s="41">
+      <c r="K30" s="32">
+        <f t="shared" ref="K30:L30" si="6">K10/K8</f>
+        <v>0.28254147485451225</v>
+      </c>
+      <c r="L30" s="32">
         <f>L10/L8</f>
         <v>0.34266327706348176</v>
       </c>
     </row>
-    <row r="31" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="41" t="s">
+    <row r="31" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="H31" s="41">
+      <c r="G31" s="32">
+        <f t="shared" ref="G31:H31" si="7">G15/G8</f>
+        <v>0.17818740399385558</v>
+      </c>
+      <c r="H31" s="32">
         <f>H15/H8</f>
         <v>-0.15928651493737533</v>
       </c>
-      <c r="L31" s="41">
+      <c r="K31" s="32">
+        <f t="shared" ref="K31:L31" si="8">K15/K8</f>
+        <v>0.1358160340484669</v>
+      </c>
+      <c r="L31" s="32">
         <f>L15/L8</f>
         <v>0.22106553029610243</v>
       </c>
     </row>
-    <row r="32" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="41" t="s">
+    <row r="32" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="H32" s="41">
+      <c r="G32" s="32">
+        <f t="shared" ref="G32:H32" si="9">G23/G8</f>
+        <v>8.5999403242383005E-2</v>
+      </c>
+      <c r="H32" s="32">
         <f>H23/H8</f>
         <v>-0.16791266630927454</v>
       </c>
-      <c r="L32" s="41">
+      <c r="K32" s="32">
+        <f t="shared" ref="K32:L32" si="10">K23/K8</f>
+        <v>-0.14563536871362814</v>
+      </c>
+      <c r="L32" s="32">
         <f>L23/L8</f>
         <v>5.2490078094992289E-3</v>
       </c>
     </row>
-    <row r="33" spans="2:12" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="41" t="s">
+    <row r="33" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="H33" s="41">
+      <c r="G33" s="32">
+        <f t="shared" ref="G33:H33" si="11">G22/G21</f>
+        <v>-0.66995708154506506</v>
+      </c>
+      <c r="H33" s="32">
         <f>H22/H21</f>
         <v>-1.0618326880206488E-2</v>
       </c>
-      <c r="L33" s="41">
+      <c r="K33" s="32">
+        <f t="shared" ref="K33:L33" si="12">K22/K21</f>
+        <v>-1.2958767557770725E-2</v>
+      </c>
+      <c r="L33" s="32">
         <f>L22/L21</f>
         <v>0.51503886448125302</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="28" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2204,7 +2359,7 @@
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="27" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2212,10 +2367,13 @@
       <c r="B41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J41" s="38">
+      <c r="J41" s="29">
         <v>132.23599999999999</v>
       </c>
-      <c r="L41" s="38">
+      <c r="K41" s="29">
+        <v>110.361</v>
+      </c>
+      <c r="L41" s="29">
         <v>79.445999999999998</v>
       </c>
     </row>
@@ -2223,10 +2381,13 @@
       <c r="B42" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J42" s="39">
-        <v>0</v>
-      </c>
-      <c r="L42" s="39">
+      <c r="J42" s="30">
+        <v>0</v>
+      </c>
+      <c r="K42" s="30">
+        <v>0</v>
+      </c>
+      <c r="L42" s="30">
         <v>10.363</v>
       </c>
     </row>
@@ -2234,10 +2395,13 @@
       <c r="B43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J43" s="38">
-        <v>0</v>
-      </c>
-      <c r="L43" s="38">
+      <c r="J43" s="29">
+        <v>0</v>
+      </c>
+      <c r="K43" s="29">
+        <v>2.9350000000000001</v>
+      </c>
+      <c r="L43" s="29">
         <v>12.125</v>
       </c>
     </row>
@@ -2245,10 +2409,13 @@
       <c r="B44" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J44" s="39">
+      <c r="J44" s="30">
         <v>5.2270000000000003</v>
       </c>
-      <c r="L44" s="39">
+      <c r="K44" s="30">
+        <v>5.431</v>
+      </c>
+      <c r="L44" s="30">
         <v>8.8070000000000004</v>
       </c>
     </row>
@@ -2256,10 +2423,13 @@
       <c r="B45" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J45" s="38">
+      <c r="J45" s="29">
         <v>10.31</v>
       </c>
-      <c r="L45" s="38">
+      <c r="K45" s="30">
+        <v>11.147</v>
+      </c>
+      <c r="L45" s="29">
         <v>11.407</v>
       </c>
     </row>
@@ -2267,10 +2437,13 @@
       <c r="B46" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J46" s="39">
+      <c r="J46" s="30">
         <v>12.731999999999999</v>
       </c>
-      <c r="L46" s="39">
+      <c r="K46" s="29">
+        <v>14.488</v>
+      </c>
+      <c r="L46" s="30">
         <v>14.206</v>
       </c>
     </row>
@@ -2278,10 +2451,13 @@
       <c r="B47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J47" s="39">
+      <c r="J47" s="30">
         <v>8.7889999999999997</v>
       </c>
-      <c r="L47" s="39">
+      <c r="K47" s="30">
+        <v>8.7189999999999994</v>
+      </c>
+      <c r="L47" s="30">
         <v>2.552</v>
       </c>
     </row>
@@ -2294,39 +2470,39 @@
         <v>0</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" ref="D48:K48" si="5">SUM(D41:D47)</f>
+        <f t="shared" ref="D48:K48" si="13">SUM(D41:D47)</f>
         <v>0</v>
       </c>
       <c r="E48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J48" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="30">
+        <f t="shared" si="13"/>
         <v>169.29399999999998</v>
       </c>
-      <c r="K48" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L48" s="39">
-        <f t="shared" ref="L48" si="6">SUM(L41:L47)</f>
+      <c r="K48" s="30">
+        <f t="shared" si="13"/>
+        <v>153.08099999999999</v>
+      </c>
+      <c r="L48" s="30">
+        <f t="shared" ref="L48" si="14">SUM(L41:L47)</f>
         <v>138.90599999999998</v>
       </c>
     </row>
@@ -2334,10 +2510,13 @@
       <c r="B49" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J49" s="39">
+      <c r="J49" s="30">
         <v>534.721</v>
       </c>
-      <c r="L49" s="39">
+      <c r="K49" s="30">
+        <v>577.26</v>
+      </c>
+      <c r="L49" s="30">
         <v>652.84699999999998</v>
       </c>
     </row>
@@ -2345,10 +2524,13 @@
       <c r="B50" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J50" s="39">
+      <c r="J50" s="30">
         <v>11.423</v>
       </c>
-      <c r="L50" s="39">
+      <c r="K50" s="30">
+        <v>12.393000000000001</v>
+      </c>
+      <c r="L50" s="30">
         <v>14.901</v>
       </c>
     </row>
@@ -2356,10 +2538,13 @@
       <c r="B51" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J51" s="39">
+      <c r="J51" s="30">
         <v>262.70299999999997</v>
       </c>
-      <c r="L51" s="39">
+      <c r="K51" s="30">
+        <v>261.61799999999999</v>
+      </c>
+      <c r="L51" s="30">
         <v>254.583</v>
       </c>
     </row>
@@ -2367,11 +2552,15 @@
       <c r="B52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J52" s="39">
+      <c r="J52" s="30">
         <f>92.593+742.669</f>
         <v>835.26199999999994</v>
       </c>
-      <c r="L52" s="39">
+      <c r="K52" s="30">
+        <f>92.119+743.655</f>
+        <v>835.774</v>
+      </c>
+      <c r="L52" s="30">
         <f>92.795+748.594</f>
         <v>841.38900000000001</v>
       </c>
@@ -2380,10 +2569,13 @@
       <c r="B53" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J53" s="39">
+      <c r="J53" s="30">
         <v>41.021999999999998</v>
       </c>
-      <c r="L53" s="39">
+      <c r="K53" s="30">
+        <v>39.341999999999999</v>
+      </c>
+      <c r="L53" s="30">
         <v>38.643000000000001</v>
       </c>
     </row>
@@ -2392,42 +2584,42 @@
         <v>94</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" ref="C54:K54" si="7">SUM(C48:C53)</f>
+        <f t="shared" ref="C54:K54" si="15">SUM(C48:C53)</f>
         <v>0</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J54" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="30">
+        <f t="shared" si="15"/>
         <v>1854.4249999999997</v>
       </c>
-      <c r="K54" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L54" s="39">
+      <c r="K54" s="30">
+        <f t="shared" si="15"/>
+        <v>1879.4680000000003</v>
+      </c>
+      <c r="L54" s="30">
         <f>SUM(L48:L53)</f>
         <v>1941.2689999999998</v>
       </c>
@@ -2436,10 +2628,13 @@
       <c r="B56" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J56" s="39">
+      <c r="J56" s="30">
         <v>38.216999999999999</v>
       </c>
-      <c r="L56" s="39">
+      <c r="K56" s="30">
+        <v>40.265000000000001</v>
+      </c>
+      <c r="L56" s="30">
         <v>44.59</v>
       </c>
     </row>
@@ -2447,10 +2642,13 @@
       <c r="B57" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J57" s="39">
+      <c r="J57" s="30">
         <v>62.853999999999999</v>
       </c>
-      <c r="L57" s="39">
+      <c r="K57" s="30">
+        <v>61.731999999999999</v>
+      </c>
+      <c r="L57" s="30">
         <v>76.611999999999995</v>
       </c>
     </row>
@@ -2458,10 +2656,13 @@
       <c r="B58" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="38">
+      <c r="J58" s="29">
         <v>4.9660000000000002</v>
       </c>
-      <c r="L58" s="38">
+      <c r="K58" s="29">
+        <v>5.8339999999999996</v>
+      </c>
+      <c r="L58" s="29">
         <v>5.8209999999999997</v>
       </c>
     </row>
@@ -2469,10 +2670,13 @@
       <c r="B59" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J59" s="39">
+      <c r="J59" s="30">
         <v>13.122999999999999</v>
       </c>
-      <c r="L59" s="39">
+      <c r="K59" s="30">
+        <v>13.906000000000001</v>
+      </c>
+      <c r="L59" s="30">
         <v>11.994999999999999</v>
       </c>
     </row>
@@ -2485,39 +2689,39 @@
         <v>0</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" ref="D60:L60" si="8">SUM(D56:D59)</f>
+        <f t="shared" ref="D60:L60" si="16">SUM(D56:D59)</f>
         <v>0</v>
       </c>
       <c r="E60" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F60" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I60" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J60" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J60" s="30">
+        <f t="shared" si="16"/>
         <v>119.16</v>
       </c>
-      <c r="K60" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L60" s="39">
-        <f t="shared" si="8"/>
+      <c r="K60" s="30">
+        <f t="shared" si="16"/>
+        <v>121.73700000000001</v>
+      </c>
+      <c r="L60" s="30">
+        <f t="shared" si="16"/>
         <v>139.018</v>
       </c>
     </row>
@@ -2525,10 +2729,13 @@
       <c r="B61" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J61" s="38">
+      <c r="J61" s="29">
         <v>865.09</v>
       </c>
-      <c r="L61" s="38">
+      <c r="K61" s="29">
+        <v>878.24300000000005</v>
+      </c>
+      <c r="L61" s="29">
         <v>876.85599999999999</v>
       </c>
     </row>
@@ -2536,10 +2743,13 @@
       <c r="B62" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J62" s="39">
+      <c r="J62" s="30">
         <v>397.60300000000001</v>
       </c>
-      <c r="L62" s="39">
+      <c r="K62" s="30">
+        <v>398.22300000000001</v>
+      </c>
+      <c r="L62" s="30">
         <v>394.83600000000001</v>
       </c>
     </row>
@@ -2547,10 +2757,13 @@
       <c r="B63" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J63" s="39">
+      <c r="J63" s="30">
         <v>210.952</v>
       </c>
-      <c r="L63" s="39">
+      <c r="K63" s="30">
+        <v>251.779</v>
+      </c>
+      <c r="L63" s="30">
         <v>282.55700000000002</v>
       </c>
     </row>
@@ -2558,10 +2771,13 @@
       <c r="B64" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J64" s="39">
+      <c r="J64" s="30">
         <v>54.417999999999999</v>
       </c>
-      <c r="L64" s="39">
+      <c r="K64" s="30">
+        <v>58.344000000000001</v>
+      </c>
+      <c r="L64" s="30">
         <v>79.353999999999999</v>
       </c>
     </row>
@@ -2569,10 +2785,13 @@
       <c r="B65" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J65" s="39">
+      <c r="J65" s="30">
         <v>14.882</v>
       </c>
-      <c r="L65" s="39">
+      <c r="K65" s="30">
+        <v>14.906000000000001</v>
+      </c>
+      <c r="L65" s="30">
         <v>15.212999999999999</v>
       </c>
     </row>
@@ -2585,51 +2804,55 @@
         <v>0</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" ref="D66:K66" si="9">SUM(D60:D65)</f>
+        <f t="shared" ref="D66:K66" si="17">SUM(D60:D65)</f>
         <v>0</v>
       </c>
       <c r="E66" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="F66" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="G66" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="H66" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I66" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="J66" s="39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="J66" s="30">
+        <f t="shared" si="17"/>
         <v>1662.105</v>
       </c>
-      <c r="K66" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L66" s="39">
-        <f t="shared" ref="L66" si="10">SUM(L60:L65)</f>
+      <c r="K66" s="30">
+        <f t="shared" si="17"/>
+        <v>1723.232</v>
+      </c>
+      <c r="L66" s="30">
+        <f t="shared" ref="L66" si="18">SUM(L60:L65)</f>
         <v>1787.8340000000001</v>
       </c>
     </row>
-    <row r="68" spans="2:12" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="39" t="s">
+    <row r="68" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J68" s="39">
+      <c r="J68" s="30">
         <f>J71</f>
         <v>192.31999999999971</v>
       </c>
-      <c r="L68" s="39">
+      <c r="K68" s="30">
+        <f t="shared" ref="K68:L68" si="19">K71</f>
+        <v>156.23600000000033</v>
+      </c>
+      <c r="L68" s="30">
         <f>L71</f>
         <v>153.43499999999972</v>
       </c>
@@ -2638,11 +2861,15 @@
       <c r="B69" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J69" s="39">
+      <c r="J69" s="30">
         <f>J68+J66</f>
         <v>1854.4249999999997</v>
       </c>
-      <c r="L69" s="39">
+      <c r="K69" s="30">
+        <f t="shared" ref="K69" si="20">K68+K66</f>
+        <v>1879.4680000000003</v>
+      </c>
+      <c r="L69" s="30">
         <f>L68+L66</f>
         <v>1941.2689999999998</v>
       </c>
@@ -2651,11 +2878,15 @@
       <c r="B71" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J71" s="39">
+      <c r="J71" s="30">
         <f>J54-J66</f>
         <v>192.31999999999971</v>
       </c>
-      <c r="L71" s="39">
+      <c r="K71" s="30">
+        <f t="shared" ref="K71:L71" si="21">K54-K66</f>
+        <v>156.23600000000033</v>
+      </c>
+      <c r="L71" s="30">
         <f>L54-L66</f>
         <v>153.43499999999972</v>
       </c>
@@ -2664,6 +2895,10 @@
       <c r="B72" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="K72" s="1">
+        <f t="shared" ref="K72" si="22">K71/K25</f>
+        <v>0.95935885678437627</v>
+      </c>
       <c r="L72" s="1">
         <f>L71/L25</f>
         <v>0.94434237977861546</v>
@@ -2673,11 +2908,15 @@
       <c r="B74" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J74" s="39">
+      <c r="J74" s="30">
         <f>J41+J43</f>
         <v>132.23599999999999</v>
       </c>
-      <c r="L74" s="39">
+      <c r="K74" s="30">
+        <f t="shared" ref="K74:L74" si="23">K41+K43</f>
+        <v>113.29600000000001</v>
+      </c>
+      <c r="L74" s="30">
         <f>L41+L43</f>
         <v>91.570999999999998</v>
       </c>
@@ -2686,11 +2925,15 @@
       <c r="B75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J75" s="39">
+      <c r="J75" s="30">
         <f>J58+J61</f>
         <v>870.05600000000004</v>
       </c>
-      <c r="L75" s="39">
+      <c r="K75" s="30">
+        <f t="shared" ref="K75:L75" si="24">K58+K61</f>
+        <v>884.077</v>
+      </c>
+      <c r="L75" s="30">
         <f>L58+L61</f>
         <v>882.67700000000002</v>
       </c>
@@ -2703,6 +2946,10 @@
         <f>J74-J75</f>
         <v>-737.82</v>
       </c>
+      <c r="K76" s="1">
+        <f t="shared" ref="K76" si="25">K74-K75</f>
+        <v>-770.78099999999995</v>
+      </c>
       <c r="L76" s="1">
         <f>L74-L75</f>
         <v>-791.10599999999999</v>
@@ -2712,38 +2959,68 @@
       <c r="B78" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="K78" s="1">
+        <v>12.66</v>
+      </c>
+      <c r="L78" s="1">
+        <v>13.72</v>
+      </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="K79" s="30">
+        <f>K78*K25</f>
+        <v>2061.73919802</v>
+      </c>
+      <c r="L79" s="30">
+        <f>L78*L25</f>
+        <v>2229.20017684</v>
+      </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="1" t="s">
+      <c r="K80" s="30">
+        <f t="shared" ref="K80" si="26">K79-K76</f>
+        <v>2832.52019802</v>
+      </c>
+      <c r="L80" s="30">
+        <f>L79-L76</f>
+        <v>3020.3061768400003</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="50" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="K82" s="50">
+        <f>K78/K72</f>
+        <v>13.196313256995801</v>
+      </c>
+      <c r="L82" s="50">
+        <f>L78/L72</f>
+        <v>14.528628910222597</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>